<commit_message>
okey I am moving forward quite a but, mean a while since my last commit but quite happy to where we are, got the betas moving on to the prediction levels.
</commit_message>
<xml_diff>
--- a/tsfl_2s_factors_correlation.xlsx
+++ b/tsfl_2s_factors_correlation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S19"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,55 +471,45 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>TSFL Small Cap</t>
+          <t>TSFL Quality</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>TSFL Quality</t>
+          <t>TSFL Low Risk</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>TSFL Low Risk</t>
+          <t>TSFL Foreign Exchange Carry</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>TSFL Foreign Exchange Carry</t>
+          <t>TSFL Fixed Income Carry</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>TSFL Fixed Income Carry</t>
+          <t>TSFL Real Estate</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>TSFL Real Estate</t>
+          <t>TSFL Currency FX</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>TSFL Currency FX</t>
+          <t>TSFL Momentum</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>TSFL Size</t>
+          <t>TSFL Value</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>TSFL Momentum</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>TSFL Value</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>TSFL Crowded</t>
         </is>
@@ -535,55 +525,49 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.1162226494997485</v>
+        <v>-0.1334416474817945</v>
       </c>
       <c r="D2" t="n">
-        <v>0.000388178490287796</v>
+        <v>0.0006285639396566115</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.001178551231457778</v>
+        <v>-0.001243277091682391</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0005736741305466983</v>
+        <v>0.0003537780769632593</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.001623592640492599</v>
+        <v>-0.001351337226277222</v>
       </c>
       <c r="H2" t="n">
-        <v>-0.000724099766245333</v>
+        <v>-0.0007988640326104693</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.00127720879204394</v>
+        <v>-0.002063876035669158</v>
       </c>
       <c r="J2" t="n">
-        <v>-0.00192218510295426</v>
+        <v>0.0006553058918174015</v>
       </c>
       <c r="K2" t="n">
-        <v>0.0001828733446477859</v>
+        <v>-0.002912955833926136</v>
       </c>
       <c r="L2" t="n">
-        <v>-0.003071584422192124</v>
+        <v>-0.001104418141534438</v>
       </c>
       <c r="M2" t="n">
-        <v>-0.001037838723109123</v>
+        <v>0.002126762259866848</v>
       </c>
       <c r="N2" t="n">
-        <v>0.00177661547466049</v>
+        <v>-0.0002844982107863287</v>
       </c>
       <c r="O2" t="n">
-        <v>-2.897294266245074e-05</v>
+        <v>-0.002361525851663136</v>
       </c>
       <c r="P2" t="n">
-        <v>0.001406589793510447</v>
+        <v>0.001141546715994384</v>
       </c>
       <c r="Q2" t="n">
-        <v>-0.002152779849852356</v>
-      </c>
-      <c r="R2" t="n">
-        <v>0.001391782568178052</v>
-      </c>
-      <c r="S2" t="n">
-        <v>-0.0001524274236050096</v>
+        <v>0.0008230026733220396</v>
       </c>
     </row>
     <row r="3">
@@ -593,58 +577,52 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.1162226494997485</v>
+        <v>-0.1334416474817945</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0001452462486910218</v>
+        <v>0.0002156854994044982</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.0004409830774835259</v>
+        <v>-0.0004266182380183484</v>
       </c>
       <c r="F3" t="n">
-        <v>0.383899447769145</v>
+        <v>0.3282120111936163</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.0006075059446486598</v>
+        <v>-0.0004636980044912222</v>
       </c>
       <c r="H3" t="n">
-        <v>-0.0002709392131639984</v>
+        <v>-0.0002741222920369469</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.0004778981589208256</v>
+        <v>-0.0007081986499356175</v>
       </c>
       <c r="J3" t="n">
-        <v>-0.0007192314424427325</v>
+        <v>0.0002248617358111303</v>
       </c>
       <c r="K3" t="n">
-        <v>6.842642742904634e-05</v>
+        <v>-0.000999551985320337</v>
       </c>
       <c r="L3" t="n">
-        <v>-0.001149306636057618</v>
+        <v>-0.000378970162588317</v>
       </c>
       <c r="M3" t="n">
-        <v>-0.0003883321334132932</v>
+        <v>0.0007297774358246361</v>
       </c>
       <c r="N3" t="n">
-        <v>0.0006647630909948505</v>
+        <v>-9.762274734825131e-05</v>
       </c>
       <c r="O3" t="n">
-        <v>-1.084091813636556e-05</v>
+        <v>-0.0008103342405417202</v>
       </c>
       <c r="P3" t="n">
-        <v>0.0005263091491837404</v>
+        <v>0.0003917104657134042</v>
       </c>
       <c r="Q3" t="n">
-        <v>-0.0008055139717247333</v>
-      </c>
-      <c r="R3" t="n">
-        <v>0.0005207686723502291</v>
-      </c>
-      <c r="S3" t="n">
-        <v>-5.703435927197228e-05</v>
+        <v>0.000282405227866728</v>
       </c>
     </row>
     <row r="4">
@@ -654,58 +632,52 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.000388178490287796</v>
+        <v>0.0006285639396566115</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0001452462486910218</v>
+        <v>0.0002156854994044982</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0.07316866887816592</v>
+        <v>0.1234611747070878</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.01536927672460082</v>
+        <v>0.1564740281543364</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0001986753805263381</v>
+        <v>0.0002261740851502603</v>
       </c>
       <c r="H4" t="n">
-        <v>8.860646014914925e-05</v>
+        <v>0.0001337063304568195</v>
       </c>
       <c r="I4" t="n">
-        <v>0.000156289167889107</v>
+        <v>0.0003454321135789705</v>
       </c>
       <c r="J4" t="n">
-        <v>0.0002352134687283961</v>
+        <v>-0.0001096789222503338</v>
       </c>
       <c r="K4" t="n">
-        <v>-2.237779996595162e-05</v>
+        <v>0.0004875430854785786</v>
       </c>
       <c r="L4" t="n">
-        <v>0.0003758628788271501</v>
+        <v>0.0001848470965855327</v>
       </c>
       <c r="M4" t="n">
-        <v>0.0001269979908120562</v>
+        <v>-0.0003559574169226238</v>
       </c>
       <c r="N4" t="n">
-        <v>-0.0002174004406484607</v>
+        <v>4.76166284034071e-05</v>
       </c>
       <c r="O4" t="n">
-        <v>3.545353843957622e-06</v>
+        <v>0.000395249933675045</v>
       </c>
       <c r="P4" t="n">
-        <v>-0.0001721212301042303</v>
+        <v>-0.0001910613273473258</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.0002634308293794042</v>
-      </c>
-      <c r="R4" t="n">
-        <v>-0.0001703093032368375</v>
-      </c>
-      <c r="S4" t="n">
-        <v>0.04985836626665967</v>
+        <v>0.1816937260702833</v>
       </c>
     </row>
     <row r="5">
@@ -715,58 +687,52 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.001178551231457778</v>
+        <v>-0.001243277091682391</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.0004409830774835259</v>
+        <v>-0.0004266182380183484</v>
       </c>
       <c r="D5" t="n">
-        <v>0.07316866887816592</v>
+        <v>0.1234611747070878</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.112373402170223</v>
+        <v>0.1788016283516784</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.0006031996111041726</v>
+        <v>-0.0004473642871610587</v>
       </c>
       <c r="H5" t="n">
-        <v>-0.0002690186482165965</v>
+        <v>-0.0002644663608302361</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.0004745105560647022</v>
+        <v>-0.0006832524210333023</v>
       </c>
       <c r="J5" t="n">
-        <v>-0.0007141331376206115</v>
+        <v>0.0002169410029301982</v>
       </c>
       <c r="K5" t="n">
-        <v>6.794138358360499e-05</v>
+        <v>-0.0009643428633771058</v>
       </c>
       <c r="L5" t="n">
-        <v>-0.001141159723647132</v>
+        <v>-0.0003656209752888468</v>
       </c>
       <c r="M5" t="n">
-        <v>-0.0003855794234070188</v>
+        <v>0.0007040710962778955</v>
       </c>
       <c r="N5" t="n">
-        <v>0.0006600508875619672</v>
+        <v>-9.418399552122308e-05</v>
       </c>
       <c r="O5" t="n">
-        <v>-1.076407179425096e-05</v>
+        <v>-0.0007817902953451855</v>
       </c>
       <c r="P5" t="n">
-        <v>0.0005225783828201919</v>
+        <v>0.0003779125024690804</v>
       </c>
       <c r="Q5" t="n">
-        <v>-0.000799804049265954</v>
-      </c>
-      <c r="R5" t="n">
-        <v>0.0005170771799088052</v>
-      </c>
-      <c r="S5" t="n">
-        <v>-0.01846398565827295</v>
+        <v>0.08552097553082703</v>
       </c>
     </row>
     <row r="6">
@@ -776,58 +742,52 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.0005736741305466983</v>
+        <v>0.0003537780769632593</v>
       </c>
       <c r="C6" t="n">
-        <v>0.383899447769145</v>
+        <v>0.3282120111936163</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.01536927672460082</v>
+        <v>0.1564740281543364</v>
       </c>
       <c r="E6" t="n">
-        <v>0.112373402170223</v>
+        <v>0.1788016283516784</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.1382032122506643</v>
+        <v>-0.2339897316267211</v>
       </c>
       <c r="H6" t="n">
-        <v>0.03635792691268026</v>
+        <v>0.02368907752826689</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.5126208873061318</v>
+        <v>0.06046630359870667</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.02976853835590626</v>
+        <v>0.174149091416109</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.07644569209598594</v>
+        <v>-0.2322558059503427</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.1352942137345701</v>
+        <v>0.04273921397679952</v>
       </c>
       <c r="M6" t="n">
-        <v>0.000603690832555673</v>
+        <v>0.05655150785596466</v>
       </c>
       <c r="N6" t="n">
-        <v>-0.07475955998194109</v>
+        <v>0.4704627725259203</v>
       </c>
       <c r="O6" t="n">
-        <v>0.3963853324106627</v>
+        <v>0.0871370607960897</v>
       </c>
       <c r="P6" t="n">
-        <v>0.07168541740254465</v>
+        <v>-0.04167564703358546</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.002468062723086028</v>
-      </c>
-      <c r="R6" t="n">
-        <v>0.01963321118563527</v>
-      </c>
-      <c r="S6" t="n">
-        <v>-0.03045858355186744</v>
+        <v>0.3277120776366273</v>
       </c>
     </row>
     <row r="7">
@@ -837,58 +797,52 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.001623592640492599</v>
+        <v>-0.001351337226277222</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.0006075059446486598</v>
+        <v>-0.0004636980044912222</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0001986753805263381</v>
+        <v>0.0002261740851502603</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.0006031996111041726</v>
+        <v>-0.0004473642871610587</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.1382032122506643</v>
+        <v>-0.2339897316267211</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>0.05080867165751436</v>
+        <v>0.05415403138743346</v>
       </c>
       <c r="I7" t="n">
-        <v>0.4421968321850102</v>
+        <v>-0.2096442069462411</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.1699368912491149</v>
+        <v>-0.1887465965667805</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.02330728570454468</v>
+        <v>0.9432299962207069</v>
       </c>
       <c r="L7" t="n">
-        <v>0.9411563061841628</v>
+        <v>-0.05626029990134487</v>
       </c>
       <c r="M7" t="n">
-        <v>-0.02995221168624869</v>
+        <v>-0.1484151694674775</v>
       </c>
       <c r="N7" t="n">
-        <v>-0.06911587491227321</v>
+        <v>-0.5074394778643724</v>
       </c>
       <c r="O7" t="n">
-        <v>-0.4755986183777171</v>
+        <v>-0.1767475188958348</v>
       </c>
       <c r="P7" t="n">
-        <v>-0.08666642010491159</v>
+        <v>-0.03978492649174577</v>
       </c>
       <c r="Q7" t="n">
-        <v>-0.1378625012925982</v>
-      </c>
-      <c r="R7" t="n">
-        <v>-0.1013733864276903</v>
-      </c>
-      <c r="S7" t="n">
-        <v>0.2195990516936987</v>
+        <v>-0.02321470386646155</v>
       </c>
     </row>
     <row r="8">
@@ -898,728 +852,546 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.000724099766245333</v>
+        <v>-0.0007988640326104693</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.0002709392131639984</v>
+        <v>-0.0002741222920369469</v>
       </c>
       <c r="D8" t="n">
-        <v>8.860646014914925e-05</v>
+        <v>0.0001337063304568195</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.0002690186482165965</v>
+        <v>-0.0002644663608302361</v>
       </c>
       <c r="F8" t="n">
-        <v>0.03635792691268026</v>
+        <v>0.02368907752826689</v>
       </c>
       <c r="G8" t="n">
-        <v>0.05080867165751436</v>
+        <v>0.05415403138743346</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>0.0116703737590046</v>
+        <v>-0.06177291002438531</v>
       </c>
       <c r="J8" t="n">
-        <v>-0.06017348341628288</v>
+        <v>-0.04343387681907708</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.040725357551785</v>
+        <v>0.08213219737675391</v>
       </c>
       <c r="L8" t="n">
-        <v>0.07947240519053494</v>
+        <v>-0.06007265100518717</v>
       </c>
       <c r="M8" t="n">
-        <v>-0.05941455482960267</v>
+        <v>0.003854908257409175</v>
       </c>
       <c r="N8" t="n">
-        <v>0.006456877052907988</v>
+        <v>-0.05498433253880837</v>
       </c>
       <c r="O8" t="n">
-        <v>-0.05240786865597571</v>
+        <v>-0.04243484380490969</v>
       </c>
       <c r="P8" t="n">
-        <v>0.05375307265546775</v>
+        <v>-0.00188418537096479</v>
       </c>
       <c r="Q8" t="n">
-        <v>-0.04086450266091254</v>
-      </c>
-      <c r="R8" t="n">
-        <v>-0.002237999533154189</v>
-      </c>
-      <c r="S8" t="n">
-        <v>0.06537229368964444</v>
+        <v>0.06168330592854031</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>TSFL Small Cap</t>
+          <t>TSFL Quality</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-0.00127720879204394</v>
+        <v>-0.002063876035669158</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.0004778981589208256</v>
+        <v>-0.0007081986499356175</v>
       </c>
       <c r="D9" t="n">
-        <v>0.000156289167889107</v>
+        <v>0.0003454321135789705</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.0004745105560647022</v>
+        <v>-0.0006832524210333023</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.5126208873061318</v>
+        <v>0.06046630359870667</v>
       </c>
       <c r="G9" t="n">
-        <v>0.4421968321850102</v>
+        <v>-0.2096442069462411</v>
       </c>
       <c r="H9" t="n">
-        <v>0.0116703737590046</v>
+        <v>-0.06177291002438531</v>
       </c>
       <c r="I9" t="n">
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>-0.1246424482488167</v>
+        <v>0.06872252418811169</v>
       </c>
       <c r="K9" t="n">
-        <v>0.04839970648359604</v>
+        <v>-0.2216672660702907</v>
       </c>
       <c r="L9" t="n">
-        <v>0.4511922587126883</v>
+        <v>-0.02869395493539544</v>
       </c>
       <c r="M9" t="n">
-        <v>0.03742174188099125</v>
+        <v>-0.01650757865824479</v>
       </c>
       <c r="N9" t="n">
-        <v>0.08864286254238694</v>
+        <v>0.1346195970889378</v>
       </c>
       <c r="O9" t="n">
-        <v>-0.3993406245194113</v>
+        <v>0.847184449957801</v>
       </c>
       <c r="P9" t="n">
-        <v>0.000566323879062398</v>
+        <v>0.0006273457161278915</v>
       </c>
       <c r="Q9" t="n">
-        <v>-0.1146484226729746</v>
-      </c>
-      <c r="R9" t="n">
-        <v>-0.1382731900474018</v>
-      </c>
-      <c r="S9" t="n">
-        <v>0.3428849234081702</v>
+        <v>-0.08433008291531877</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>TSFL Quality</t>
+          <t>TSFL Low Risk</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-0.00192218510295426</v>
+        <v>0.0006553058918174015</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.0007192314424427325</v>
+        <v>0.0002248617358111303</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0002352134687283961</v>
+        <v>-0.0001096789222503338</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.0007141331376206115</v>
+        <v>0.0002169410029301982</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.02976853835590626</v>
+        <v>0.174149091416109</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.1699368912491149</v>
+        <v>-0.1887465965667805</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.06017348341628288</v>
+        <v>-0.04343387681907708</v>
       </c>
       <c r="I10" t="n">
-        <v>-0.1246424482488167</v>
+        <v>0.06872252418811169</v>
       </c>
       <c r="J10" t="n">
         <v>1</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.01509755565636652</v>
+        <v>-0.1713373731830908</v>
       </c>
       <c r="L10" t="n">
-        <v>-0.1829458446989566</v>
+        <v>0.1583397734561896</v>
       </c>
       <c r="M10" t="n">
-        <v>-0.04473831764623552</v>
+        <v>0.4067210804747039</v>
       </c>
       <c r="N10" t="n">
-        <v>-0.06323259384088402</v>
+        <v>0.1678789684238447</v>
       </c>
       <c r="O10" t="n">
-        <v>0.08353701694989403</v>
+        <v>0.0484875118390069</v>
       </c>
       <c r="P10" t="n">
-        <v>0.0231682415714996</v>
+        <v>0.4856746049480272</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.8459574185383545</v>
-      </c>
-      <c r="R10" t="n">
-        <v>0.0008433388602624184</v>
-      </c>
-      <c r="S10" t="n">
-        <v>-0.09990904576090746</v>
+        <v>-0.2483500861966133</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>TSFL Low Risk</t>
+          <t>TSFL Foreign Exchange Carry</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.0001828733446477859</v>
+        <v>-0.002912955833926136</v>
       </c>
       <c r="C11" t="n">
-        <v>6.842642742904634e-05</v>
+        <v>-0.000999551985320337</v>
       </c>
       <c r="D11" t="n">
-        <v>-2.237779996595162e-05</v>
+        <v>0.0004875430854785786</v>
       </c>
       <c r="E11" t="n">
-        <v>6.794138358360499e-05</v>
+        <v>-0.0009643428633771058</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.07644569209598594</v>
+        <v>-0.2322558059503427</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.02330728570454468</v>
+        <v>0.9432299962207069</v>
       </c>
       <c r="H11" t="n">
-        <v>-0.040725357551785</v>
+        <v>0.08213219737675391</v>
       </c>
       <c r="I11" t="n">
-        <v>0.04839970648359604</v>
+        <v>-0.2216672660702907</v>
       </c>
       <c r="J11" t="n">
-        <v>-0.01509755565636652</v>
+        <v>-0.1713373731830908</v>
       </c>
       <c r="K11" t="n">
         <v>1</v>
       </c>
       <c r="L11" t="n">
-        <v>-0.007142045507600501</v>
+        <v>-0.06875756420503713</v>
       </c>
       <c r="M11" t="n">
-        <v>0.142034087885073</v>
+        <v>-0.1360525844712651</v>
       </c>
       <c r="N11" t="n">
-        <v>0.3747888393308351</v>
+        <v>-0.5108036084660109</v>
       </c>
       <c r="O11" t="n">
-        <v>-0.005814810407884411</v>
+        <v>-0.1928415697718273</v>
       </c>
       <c r="P11" t="n">
-        <v>-0.1506668545305144</v>
+        <v>-0.02502062945466294</v>
       </c>
       <c r="Q11" t="n">
-        <v>-0.02632932145390253</v>
-      </c>
-      <c r="R11" t="n">
-        <v>0.4832907203989945</v>
-      </c>
-      <c r="S11" t="n">
-        <v>-0.3714135833417243</v>
+        <v>-0.0320552259653662</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>TSFL Foreign Exchange Carry</t>
+          <t>TSFL Fixed Income Carry</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0.003071584422192124</v>
+        <v>-0.001104418141534438</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.001149306636057618</v>
+        <v>-0.000378970162588317</v>
       </c>
       <c r="D12" t="n">
-        <v>0.0003758628788271501</v>
+        <v>0.0001848470965855327</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.001141159723647132</v>
+        <v>-0.0003656209752888468</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.1352942137345701</v>
+        <v>0.04273921397679952</v>
       </c>
       <c r="G12" t="n">
-        <v>0.9411563061841628</v>
+        <v>-0.05626029990134487</v>
       </c>
       <c r="H12" t="n">
-        <v>0.07947240519053494</v>
+        <v>-0.06007265100518717</v>
       </c>
       <c r="I12" t="n">
-        <v>0.4511922587126883</v>
+        <v>-0.02869395493539544</v>
       </c>
       <c r="J12" t="n">
-        <v>-0.1829458446989566</v>
+        <v>0.1583397734561896</v>
       </c>
       <c r="K12" t="n">
-        <v>-0.007142045507600501</v>
+        <v>-0.06875756420503713</v>
       </c>
       <c r="L12" t="n">
         <v>1</v>
       </c>
       <c r="M12" t="n">
-        <v>-0.04302754595115078</v>
+        <v>0.1845941818018214</v>
       </c>
       <c r="N12" t="n">
-        <v>-0.05750735067313216</v>
+        <v>0.04720658872404225</v>
       </c>
       <c r="O12" t="n">
-        <v>-0.4789847991294744</v>
+        <v>-0.04303048941189345</v>
       </c>
       <c r="P12" t="n">
-        <v>-0.09844105470561677</v>
+        <v>0.1121570486383558</v>
       </c>
       <c r="Q12" t="n">
-        <v>-0.1546818500971746</v>
-      </c>
-      <c r="R12" t="n">
-        <v>-0.08499078023261446</v>
-      </c>
-      <c r="S12" t="n">
-        <v>0.2044494140890493</v>
+        <v>-0.04715686835536838</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>TSFL Fixed Income Carry</t>
+          <t>TSFL Real Estate</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-0.001037838723109123</v>
+        <v>0.002126762259866848</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.0003883321334132932</v>
+        <v>0.0007297774358246361</v>
       </c>
       <c r="D13" t="n">
-        <v>0.0001269979908120562</v>
+        <v>-0.0003559574169226238</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.0003855794234070188</v>
+        <v>0.0007040710962778955</v>
       </c>
       <c r="F13" t="n">
-        <v>0.000603690832555673</v>
+        <v>0.05655150785596466</v>
       </c>
       <c r="G13" t="n">
-        <v>-0.02995221168624869</v>
+        <v>-0.1484151694674775</v>
       </c>
       <c r="H13" t="n">
-        <v>-0.05941455482960267</v>
+        <v>0.003854908257409175</v>
       </c>
       <c r="I13" t="n">
-        <v>0.03742174188099125</v>
+        <v>-0.01650757865824479</v>
       </c>
       <c r="J13" t="n">
-        <v>-0.04473831764623552</v>
+        <v>0.4067210804747039</v>
       </c>
       <c r="K13" t="n">
-        <v>0.142034087885073</v>
+        <v>-0.1360525844712651</v>
       </c>
       <c r="L13" t="n">
-        <v>-0.04302754595115078</v>
+        <v>0.1845941818018214</v>
       </c>
       <c r="M13" t="n">
         <v>1</v>
       </c>
       <c r="N13" t="n">
-        <v>0.1748414340378834</v>
+        <v>0.1337417756014269</v>
       </c>
       <c r="O13" t="n">
-        <v>0.01888068254919643</v>
+        <v>-0.1096864362860457</v>
       </c>
       <c r="P13" t="n">
-        <v>-0.08468423638430531</v>
+        <v>0.4428383113970458</v>
       </c>
       <c r="Q13" t="n">
-        <v>-0.05805056344233685</v>
-      </c>
-      <c r="R13" t="n">
-        <v>0.1114237283502749</v>
-      </c>
-      <c r="S13" t="n">
-        <v>-0.08303218850690249</v>
+        <v>-0.05648352100553627</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>TSFL Real Estate</t>
+          <t>TSFL Currency FX</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.00177661547466049</v>
+        <v>-0.0002844982107863287</v>
       </c>
       <c r="C14" t="n">
-        <v>0.0006647630909948505</v>
+        <v>-9.762274734825131e-05</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.0002174004406484607</v>
+        <v>4.76166284034071e-05</v>
       </c>
       <c r="E14" t="n">
-        <v>0.0006600508875619672</v>
+        <v>-9.418399552122308e-05</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.07475955998194109</v>
+        <v>0.4704627725259203</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.06911587491227321</v>
+        <v>-0.5074394778643724</v>
       </c>
       <c r="H14" t="n">
-        <v>0.006456877052907988</v>
+        <v>-0.05498433253880837</v>
       </c>
       <c r="I14" t="n">
-        <v>0.08864286254238694</v>
+        <v>0.1346195970889378</v>
       </c>
       <c r="J14" t="n">
-        <v>-0.06323259384088402</v>
+        <v>0.1678789684238447</v>
       </c>
       <c r="K14" t="n">
-        <v>0.3747888393308351</v>
+        <v>-0.5108036084660109</v>
       </c>
       <c r="L14" t="n">
-        <v>-0.05750735067313216</v>
+        <v>0.04720658872404225</v>
       </c>
       <c r="M14" t="n">
-        <v>0.1748414340378834</v>
+        <v>0.1337417756014269</v>
       </c>
       <c r="N14" t="n">
         <v>1</v>
       </c>
       <c r="O14" t="n">
-        <v>0.05120807136413843</v>
+        <v>0.1117556967797009</v>
       </c>
       <c r="P14" t="n">
-        <v>0.2519390374675503</v>
+        <v>0.06746041205686211</v>
       </c>
       <c r="Q14" t="n">
-        <v>-0.1514040660012911</v>
-      </c>
-      <c r="R14" t="n">
-        <v>0.435657264703426</v>
-      </c>
-      <c r="S14" t="n">
-        <v>-0.1301434950242978</v>
+        <v>0.1098460410043532</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>TSFL Currency FX</t>
+          <t>TSFL Momentum</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-2.897294266245074e-05</v>
+        <v>-0.002361525851663136</v>
       </c>
       <c r="C15" t="n">
-        <v>-1.084091813636556e-05</v>
+        <v>-0.0008103342405417202</v>
       </c>
       <c r="D15" t="n">
-        <v>3.545353843957622e-06</v>
+        <v>0.000395249933675045</v>
       </c>
       <c r="E15" t="n">
-        <v>-1.076407179425096e-05</v>
+        <v>-0.0007817902953451855</v>
       </c>
       <c r="F15" t="n">
-        <v>0.3963853324106627</v>
+        <v>0.0871370607960897</v>
       </c>
       <c r="G15" t="n">
-        <v>-0.4755986183777171</v>
+        <v>-0.1767475188958348</v>
       </c>
       <c r="H15" t="n">
-        <v>-0.05240786865597571</v>
+        <v>-0.04243484380490969</v>
       </c>
       <c r="I15" t="n">
-        <v>-0.3993406245194113</v>
+        <v>0.847184449957801</v>
       </c>
       <c r="J15" t="n">
-        <v>0.08353701694989403</v>
+        <v>0.0484875118390069</v>
       </c>
       <c r="K15" t="n">
-        <v>-0.005814810407884411</v>
+        <v>-0.1928415697718273</v>
       </c>
       <c r="L15" t="n">
-        <v>-0.4789847991294744</v>
+        <v>-0.04303048941189345</v>
       </c>
       <c r="M15" t="n">
-        <v>0.01888068254919643</v>
+        <v>-0.1096864362860457</v>
       </c>
       <c r="N15" t="n">
-        <v>0.05120807136413843</v>
+        <v>0.1117556967797009</v>
       </c>
       <c r="O15" t="n">
         <v>1</v>
       </c>
       <c r="P15" t="n">
-        <v>0.1120816215681397</v>
+        <v>-0.1665988250978098</v>
       </c>
       <c r="Q15" t="n">
-        <v>0.06183242663445167</v>
-      </c>
-      <c r="R15" t="n">
-        <v>0.1248628874492944</v>
-      </c>
-      <c r="S15" t="n">
-        <v>-0.1356683405571987</v>
+        <v>0.0005175157713028264</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>TSFL Size</t>
+          <t>TSFL Value</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.001406589793510447</v>
+        <v>0.001141546715994384</v>
       </c>
       <c r="C16" t="n">
-        <v>0.0005263091491837404</v>
+        <v>0.0003917104657134042</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.0001721212301042303</v>
+        <v>-0.0001910613273473258</v>
       </c>
       <c r="E16" t="n">
-        <v>0.0005225783828201919</v>
+        <v>0.0003779125024690804</v>
       </c>
       <c r="F16" t="n">
-        <v>0.07168541740254465</v>
+        <v>-0.04167564703358546</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.08666642010491159</v>
+        <v>-0.03978492649174577</v>
       </c>
       <c r="H16" t="n">
-        <v>0.05375307265546775</v>
+        <v>-0.00188418537096479</v>
       </c>
       <c r="I16" t="n">
-        <v>0.000566323879062398</v>
+        <v>0.0006273457161278915</v>
       </c>
       <c r="J16" t="n">
-        <v>0.0231682415714996</v>
+        <v>0.4856746049480272</v>
       </c>
       <c r="K16" t="n">
-        <v>-0.1506668545305144</v>
+        <v>-0.02502062945466294</v>
       </c>
       <c r="L16" t="n">
-        <v>-0.09844105470561677</v>
+        <v>0.1121570486383558</v>
       </c>
       <c r="M16" t="n">
-        <v>-0.08468423638430531</v>
+        <v>0.4428383113970458</v>
       </c>
       <c r="N16" t="n">
-        <v>0.2519390374675503</v>
+        <v>0.06746041205686211</v>
       </c>
       <c r="O16" t="n">
-        <v>0.1120816215681397</v>
+        <v>-0.1665988250978098</v>
       </c>
       <c r="P16" t="n">
         <v>1</v>
       </c>
       <c r="Q16" t="n">
-        <v>-0.0227060320173561</v>
-      </c>
-      <c r="R16" t="n">
-        <v>0.3143838309701617</v>
-      </c>
-      <c r="S16" t="n">
-        <v>0.2300933913935983</v>
+        <v>-0.3242089088795631</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>TSFL Momentum</t>
+          <t>TSFL Crowded</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.002152779849852356</v>
+        <v>0.0008230026733220396</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.0008055139717247333</v>
+        <v>0.000282405227866728</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0002634308293794042</v>
+        <v>0.1816937260702833</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.000799804049265954</v>
+        <v>0.08552097553082703</v>
       </c>
       <c r="F17" t="n">
-        <v>0.002468062723086028</v>
+        <v>0.3277120776366273</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.1378625012925982</v>
+        <v>-0.02321470386646155</v>
       </c>
       <c r="H17" t="n">
-        <v>-0.04086450266091254</v>
+        <v>0.06168330592854031</v>
       </c>
       <c r="I17" t="n">
-        <v>-0.1146484226729746</v>
+        <v>-0.08433008291531877</v>
       </c>
       <c r="J17" t="n">
-        <v>0.8459574185383545</v>
+        <v>-0.2483500861966133</v>
       </c>
       <c r="K17" t="n">
-        <v>-0.02632932145390253</v>
+        <v>-0.0320552259653662</v>
       </c>
       <c r="L17" t="n">
-        <v>-0.1546818500971746</v>
+        <v>-0.04715686835536838</v>
       </c>
       <c r="M17" t="n">
-        <v>-0.05805056344233685</v>
+        <v>-0.05648352100553627</v>
       </c>
       <c r="N17" t="n">
-        <v>-0.1514040660012911</v>
+        <v>0.1098460410043532</v>
       </c>
       <c r="O17" t="n">
-        <v>0.06183242663445167</v>
+        <v>0.0005175157713028264</v>
       </c>
       <c r="P17" t="n">
-        <v>-0.0227060320173561</v>
+        <v>-0.3242089088795631</v>
       </c>
       <c r="Q17" t="n">
-        <v>1</v>
-      </c>
-      <c r="R17" t="n">
-        <v>-0.1494992119030372</v>
-      </c>
-      <c r="S17" t="n">
-        <v>-0.0001034423174537139</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="inlineStr">
-        <is>
-          <t>TSFL Value</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>0.001391782568178052</v>
-      </c>
-      <c r="C18" t="n">
-        <v>0.0005207686723502291</v>
-      </c>
-      <c r="D18" t="n">
-        <v>-0.0001703093032368375</v>
-      </c>
-      <c r="E18" t="n">
-        <v>0.0005170771799088052</v>
-      </c>
-      <c r="F18" t="n">
-        <v>0.01963321118563527</v>
-      </c>
-      <c r="G18" t="n">
-        <v>-0.1013733864276903</v>
-      </c>
-      <c r="H18" t="n">
-        <v>-0.002237999533154189</v>
-      </c>
-      <c r="I18" t="n">
-        <v>-0.1382731900474018</v>
-      </c>
-      <c r="J18" t="n">
-        <v>0.0008433388602624184</v>
-      </c>
-      <c r="K18" t="n">
-        <v>0.4832907203989945</v>
-      </c>
-      <c r="L18" t="n">
-        <v>-0.08499078023261446</v>
-      </c>
-      <c r="M18" t="n">
-        <v>0.1114237283502749</v>
-      </c>
-      <c r="N18" t="n">
-        <v>0.435657264703426</v>
-      </c>
-      <c r="O18" t="n">
-        <v>0.1248628874492944</v>
-      </c>
-      <c r="P18" t="n">
-        <v>0.3143838309701617</v>
-      </c>
-      <c r="Q18" t="n">
-        <v>-0.1494992119030372</v>
-      </c>
-      <c r="R18" t="n">
-        <v>1</v>
-      </c>
-      <c r="S18" t="n">
-        <v>-0.4075982369234768</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="inlineStr">
-        <is>
-          <t>TSFL Crowded</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>-0.0001524274236050096</v>
-      </c>
-      <c r="C19" t="n">
-        <v>-5.703435927197228e-05</v>
-      </c>
-      <c r="D19" t="n">
-        <v>0.04985836626665967</v>
-      </c>
-      <c r="E19" t="n">
-        <v>-0.01846398565827295</v>
-      </c>
-      <c r="F19" t="n">
-        <v>-0.03045858355186744</v>
-      </c>
-      <c r="G19" t="n">
-        <v>0.2195990516936987</v>
-      </c>
-      <c r="H19" t="n">
-        <v>0.06537229368964444</v>
-      </c>
-      <c r="I19" t="n">
-        <v>0.3428849234081702</v>
-      </c>
-      <c r="J19" t="n">
-        <v>-0.09990904576090746</v>
-      </c>
-      <c r="K19" t="n">
-        <v>-0.3714135833417243</v>
-      </c>
-      <c r="L19" t="n">
-        <v>0.2044494140890493</v>
-      </c>
-      <c r="M19" t="n">
-        <v>-0.08303218850690249</v>
-      </c>
-      <c r="N19" t="n">
-        <v>-0.1301434950242978</v>
-      </c>
-      <c r="O19" t="n">
-        <v>-0.1356683405571987</v>
-      </c>
-      <c r="P19" t="n">
-        <v>0.2300933913935983</v>
-      </c>
-      <c r="Q19" t="n">
-        <v>-0.0001034423174537139</v>
-      </c>
-      <c r="R19" t="n">
-        <v>-0.4075982369234768</v>
-      </c>
-      <c r="S19" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>